<commit_message>
Updates to temperature application and tableManipulator
</commit_message>
<xml_diff>
--- a/Applications/Arduino/Simulink/TemperatureControl/Step02_OpenLoop/OpenLoopRunIDs.xlsx
+++ b/Applications/Arduino/Simulink/TemperatureControl/Step02_OpenLoop/OpenLoopRunIDs.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MatlabLum\Applications\Arduino\Simulink\TemperatureControl\Step02_OpenLoop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B61521A-D2F8-43FE-9F8C-6A76352CF6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3626F05-66FC-4D28-B720-7F7F3B6D72EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="-15915" windowWidth="21075" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>File</t>
   </si>
@@ -73,6 +84,24 @@
   </si>
   <si>
     <t>OpenLoopSimulinkData_ID07</t>
+  </si>
+  <si>
+    <t>Constant duty cycle input, used for system ID</t>
+  </si>
+  <si>
+    <t>OpenLoopSimulinkData_ID08</t>
+  </si>
+  <si>
+    <t>OpenLoopSimulinkData_ID09</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>with fan on low but close to heater</t>
+  </si>
+  <si>
+    <t>open loop run (in box)</t>
   </si>
 </sst>
 </file>
@@ -412,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +496,9 @@
       <c r="F2" s="3">
         <v>45668</v>
       </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -487,6 +519,9 @@
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -507,6 +542,9 @@
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -527,6 +565,9 @@
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -547,6 +588,9 @@
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -567,6 +611,9 @@
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -589,6 +636,52 @@
       </c>
       <c r="G8" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>900</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>